<commit_message>
Fatto la funzione Matlab
Dovrebbe funzionare quasi perfettamente, i risultati si discostano di pochissimo da quelli segnati sulle slide con la rete che ho provato
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365-my.sharepoint.com/personal/10014853_polimi_it/Documents/Electric Power Systems/2025-2026/Progetti/Project 01/Vediamo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365-my.sharepoint.com/personal/10834079_polimi_it/Documents/Quarto anno/Primo semestre/EPS/Projects/Project 1 - Power Flow Analysis/ProgettoEPS1/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="416" documentId="11_AD4DB114E441178AC67DF40BBED6E3B2683EDF25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E0AD0B2-DA06-478B-9245-07CE4659C77A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25420" windowHeight="16300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -276,10 +276,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -547,20 +543,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -583,7 +579,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -606,7 +602,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -629,7 +625,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -652,7 +648,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -675,7 +671,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -698,7 +694,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -721,7 +717,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -744,7 +740,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -767,7 +763,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -790,7 +786,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -813,7 +809,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -836,7 +832,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -859,7 +855,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -882,7 +878,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -915,21 +911,21 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U24" sqref="U24:U26"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -964,7 +960,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -999,7 +995,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1034,7 +1030,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1069,7 +1065,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1104,7 +1100,7 @@
         <v>44.1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1149,21 +1145,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9613FA2B-04AF-4B9C-9194-CAAD402285D2}">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.26953125" customWidth="1"/>
     <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -1207,7 +1203,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1248,7 +1244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1289,7 +1285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1330,7 +1326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1371,7 +1367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1412,7 +1408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1453,7 +1449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1494,7 +1490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>4</v>
       </c>
@@ -1538,7 +1534,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>4</v>
       </c>
@@ -1582,7 +1578,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>5</v>
       </c>
@@ -1626,7 +1622,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>6</v>
       </c>
@@ -1667,7 +1663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>6</v>
       </c>
@@ -1708,7 +1704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>6</v>
       </c>
@@ -1749,7 +1745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>7</v>
       </c>
@@ -1793,7 +1789,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>7</v>
       </c>
@@ -1834,7 +1830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>9</v>
       </c>
@@ -1875,7 +1871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>9</v>
       </c>
@@ -1916,7 +1912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>10</v>
       </c>
@@ -1957,7 +1953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>12</v>
       </c>
@@ -1998,7 +1994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>13</v>
       </c>
@@ -2049,15 +2045,15 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2068,7 +2064,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>4</v>
       </c>
@@ -2079,7 +2075,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>9</v>
       </c>
@@ -2090,7 +2086,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>12</v>
       </c>
@@ -2111,17 +2107,17 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:I15"/>
+      <selection activeCell="M25" sqref="F25:M39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2132,7 +2128,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2143,7 +2139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2154,7 +2150,7 @@
         <v>-4.9564700000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2165,7 +2161,7 @@
         <v>-12.63274</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2176,7 +2172,7 @@
         <v>-10.36585</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2187,7 +2183,7 @@
         <v>-8.9466300000000007</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2198,7 +2194,7 @@
         <v>-14.87918</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2209,7 +2205,7 @@
         <v>-13.45011</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2220,7 +2216,7 @@
         <v>-13.450049999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2231,7 +2227,7 @@
         <v>-15.06968</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2242,7 +2238,7 @@
         <v>-15.31793</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2253,7 +2249,7 @@
         <v>-15.213240000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2264,7 +2260,7 @@
         <v>-15.719469999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2275,7 +2271,7 @@
         <v>-15.738060000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Tabella per punto 9
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365-my.sharepoint.com/personal/10834079_polimi_it/Documents/Quarto anno/Primo semestre/EPS/Projects/Project 1 - Power Flow Analysis/ProgettoEPS1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshu.THINKJOSHUA\Desktop\ProgettoEPS1\ProgettoEPS1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="567" documentId="11_AD4DB114E441178AC67DF40BBED6E3B2683EDF25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAE96CF1-A992-4950-B5F3-CE9801926F5E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC837FA-ED65-4767-9870-5457D25183E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25420" windowHeight="16300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Shunt capacitors" sheetId="4" r:id="rId4"/>
     <sheet name="PF results (NR)" sheetId="5" r:id="rId5"/>
     <sheet name="Sensitività" sheetId="6" r:id="rId6"/>
+    <sheet name="Capacitors" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="64">
   <si>
     <t>Node</t>
   </si>
@@ -218,6 +219,45 @@
   <si>
     <t>Angles</t>
   </si>
+  <si>
+    <t>losses</t>
+  </si>
+  <si>
+    <t>c 1</t>
+  </si>
+  <si>
+    <t>c closed</t>
+  </si>
+  <si>
+    <t>c2</t>
+  </si>
+  <si>
+    <t>c3</t>
+  </si>
+  <si>
+    <t>bus</t>
+  </si>
+  <si>
+    <t>c1 c3</t>
+  </si>
+  <si>
+    <t>c2 c1</t>
+  </si>
+  <si>
+    <t>teniamo chiuso il 9 pk è lunico che diminuisce</t>
+  </si>
+  <si>
+    <t>c2 c3</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
+  <si>
+    <t>somma δ</t>
+  </si>
+  <si>
+    <t>valore iniziale</t>
+  </si>
 </sst>
 </file>
 
@@ -263,10 +303,36 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -275,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -284,6 +350,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -3962,16 +4030,16 @@
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3994,7 +4062,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4017,7 +4085,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4040,7 +4108,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4063,7 +4131,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4086,7 +4154,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4109,7 +4177,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4132,7 +4200,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4155,7 +4223,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4178,7 +4246,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4201,7 +4269,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4224,7 +4292,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4247,7 +4315,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4270,7 +4338,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4293,7 +4361,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4329,18 +4397,18 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -4375,7 +4443,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4410,7 +4478,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4445,7 +4513,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4480,7 +4548,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4515,7 +4583,7 @@
         <v>44.1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4564,17 +4632,17 @@
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.26953125" customWidth="1"/>
+    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.21875" customWidth="1"/>
     <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -4618,7 +4686,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4659,7 +4727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4700,7 +4768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -4741,7 +4809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -4782,7 +4850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -4823,7 +4891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3</v>
       </c>
@@ -4864,7 +4932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>4</v>
       </c>
@@ -4905,7 +4973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>4</v>
       </c>
@@ -4949,7 +5017,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>4</v>
       </c>
@@ -4993,7 +5061,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>5</v>
       </c>
@@ -5037,7 +5105,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>6</v>
       </c>
@@ -5078,7 +5146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>6</v>
       </c>
@@ -5119,7 +5187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>6</v>
       </c>
@@ -5160,7 +5228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>7</v>
       </c>
@@ -5204,7 +5272,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>7</v>
       </c>
@@ -5245,7 +5313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>9</v>
       </c>
@@ -5286,7 +5354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>9</v>
       </c>
@@ -5327,7 +5395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>10</v>
       </c>
@@ -5368,7 +5436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>12</v>
       </c>
@@ -5409,7 +5477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>13</v>
       </c>
@@ -5463,12 +5531,12 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -5479,7 +5547,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>4</v>
       </c>
@@ -5490,7 +5558,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>9</v>
       </c>
@@ -5501,7 +5569,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>12</v>
       </c>
@@ -5525,14 +5593,14 @@
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5543,7 +5611,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5554,7 +5622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5565,7 +5633,7 @@
         <v>-4.9564700000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5576,7 +5644,7 @@
         <v>-12.63274</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5587,7 +5655,7 @@
         <v>-10.36585</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5598,7 +5666,7 @@
         <v>-8.9466300000000007</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5609,7 +5677,7 @@
         <v>-14.87918</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -5620,7 +5688,7 @@
         <v>-13.45011</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -5631,7 +5699,7 @@
         <v>-13.450049999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5642,7 +5710,7 @@
         <v>-15.06968</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -5653,7 +5721,7 @@
         <v>-15.31793</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -5664,7 +5732,7 @@
         <v>-15.213240000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -5675,7 +5743,7 @@
         <v>-15.719469999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -5686,7 +5754,7 @@
         <v>-15.738060000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -5706,13 +5774,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E66A2649-79A9-4750-81F8-F6613BFE84EB}">
   <dimension ref="C4:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>50</v>
       </c>
@@ -5723,7 +5791,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D5" s="3" t="s">
         <v>45</v>
       </c>
@@ -5737,7 +5805,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C6">
         <v>0</v>
       </c>
@@ -5751,7 +5819,7 @@
         <v>72.599999999999994</v>
       </c>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C7">
         <f>C6+2</f>
         <v>2</v>
@@ -5766,9 +5834,9 @@
         <v>72.900000000000006</v>
       </c>
     </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C8">
-        <f t="shared" ref="C8:C22" si="0">C7+2</f>
+        <f t="shared" ref="C8:C21" si="0">C7+2</f>
         <v>4</v>
       </c>
       <c r="D8">
@@ -5781,7 +5849,7 @@
         <v>73.099999999999994</v>
       </c>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C9">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -5796,7 +5864,7 @@
         <v>73.400000000000006</v>
       </c>
     </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -5811,7 +5879,7 @@
         <v>73.7</v>
       </c>
     </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -5826,7 +5894,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C12">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -5841,7 +5909,7 @@
         <v>74.3</v>
       </c>
     </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C13">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -5856,7 +5924,7 @@
         <v>74.599999999999994</v>
       </c>
     </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C14">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -5871,7 +5939,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C15">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -5886,7 +5954,7 @@
         <v>75.400000000000006</v>
       </c>
     </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C16">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -5901,7 +5969,7 @@
         <v>75.8</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C17">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -5916,7 +5984,7 @@
         <v>76.2</v>
       </c>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C18">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -5931,7 +5999,7 @@
         <v>76.599999999999994</v>
       </c>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C19">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -5946,7 +6014,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C20">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -5961,7 +6029,7 @@
         <v>77.5</v>
       </c>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C21">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -5976,7 +6044,7 @@
         <v>77.900000000000006</v>
       </c>
     </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C22">
         <v>-2</v>
       </c>
@@ -5990,7 +6058,7 @@
         <v>72.400000000000006</v>
       </c>
     </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C23">
         <f>C22-2</f>
         <v>-4</v>
@@ -6005,9 +6073,9 @@
         <v>72.2</v>
       </c>
     </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C24">
-        <f t="shared" ref="C24:C38" si="1">C23-2</f>
+        <f t="shared" ref="C24:C36" si="1">C23-2</f>
         <v>-6</v>
       </c>
       <c r="D24">
@@ -6020,7 +6088,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C25">
         <f t="shared" si="1"/>
         <v>-8</v>
@@ -6035,7 +6103,7 @@
         <v>71.8</v>
       </c>
     </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C26">
         <f t="shared" si="1"/>
         <v>-10</v>
@@ -6050,7 +6118,7 @@
         <v>71.599999999999994</v>
       </c>
     </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C27">
         <f t="shared" si="1"/>
         <v>-12</v>
@@ -6065,7 +6133,7 @@
         <v>71.400000000000006</v>
       </c>
     </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C28">
         <f t="shared" si="1"/>
         <v>-14</v>
@@ -6080,7 +6148,7 @@
         <v>71.3</v>
       </c>
     </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C29">
         <f t="shared" si="1"/>
         <v>-16</v>
@@ -6095,7 +6163,7 @@
         <v>71.2</v>
       </c>
     </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C30">
         <f t="shared" si="1"/>
         <v>-18</v>
@@ -6110,7 +6178,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C31">
         <f t="shared" si="1"/>
         <v>-20</v>
@@ -6125,7 +6193,7 @@
         <v>70.900000000000006</v>
       </c>
     </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C32">
         <f t="shared" si="1"/>
         <v>-22</v>
@@ -6140,7 +6208,7 @@
         <v>70.8</v>
       </c>
     </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C33">
         <f t="shared" si="1"/>
         <v>-24</v>
@@ -6155,7 +6223,7 @@
         <v>70.8</v>
       </c>
     </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C34">
         <f t="shared" si="1"/>
         <v>-26</v>
@@ -6170,7 +6238,7 @@
         <v>70.8</v>
       </c>
     </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C35">
         <f t="shared" si="1"/>
         <v>-28</v>
@@ -6185,7 +6253,7 @@
         <v>70.8</v>
       </c>
     </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C36">
         <f t="shared" si="1"/>
         <v>-30</v>
@@ -6204,4 +6272,150 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95A985C-9000-4D98-9A41-CFC91BE0E4F9}">
+  <dimension ref="D3:I12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="12.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="I3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="F4" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="4">
+        <v>6.96</v>
+      </c>
+    </row>
+    <row r="6" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D6" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D7" s="4">
+        <v>4</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="4">
+        <v>6.99</v>
+      </c>
+      <c r="G7" s="4">
+        <f>F7-$G$4</f>
+        <v>3.0000000000000249E-2</v>
+      </c>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D8" s="4">
+        <v>9</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="4">
+        <v>6.79</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" ref="G8:G12" si="0">F8-$G$4</f>
+        <v>-0.16999999999999993</v>
+      </c>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D9" s="4">
+        <v>12</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="4">
+        <v>7.26</v>
+      </c>
+      <c r="G9" s="4">
+        <f t="shared" si="0"/>
+        <v>0.29999999999999982</v>
+      </c>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="4">
+        <v>6.89</v>
+      </c>
+      <c r="G10" s="4">
+        <f t="shared" si="0"/>
+        <v>-7.0000000000000284E-2</v>
+      </c>
+      <c r="H10" s="4">
+        <f>G7+G8</f>
+        <v>-0.13999999999999968</v>
+      </c>
+    </row>
+    <row r="11" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D11" s="4"/>
+      <c r="E11" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="4">
+        <v>7.1</v>
+      </c>
+      <c r="G11" s="4">
+        <f t="shared" si="0"/>
+        <v>0.13999999999999968</v>
+      </c>
+      <c r="H11" s="4">
+        <f>G8+G9</f>
+        <v>0.12999999999999989</v>
+      </c>
+    </row>
+    <row r="12" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="E12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="5">
+        <v>7.3</v>
+      </c>
+      <c r="G12" s="5">
+        <f t="shared" si="0"/>
+        <v>0.33999999999999986</v>
+      </c>
+      <c r="H12" s="4">
+        <f>G7+G9</f>
+        <v>0.33000000000000007</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Spoiler: non era finito
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365-my.sharepoint.com/personal/10834079_polimi_it/Documents/Quarto anno/Primo semestre/EPS/Projects/Project 1 - Power Flow Analysis/ProgettoEPS1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{3CC837FA-ED65-4767-9870-5457D25183E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6970C72-4D8D-4C5F-8EFF-1AAD59E601D3}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="13_ncr:1_{3CC837FA-ED65-4767-9870-5457D25183E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6674D1C8-4C85-4FBA-8034-BF328B3DE5B2}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25420" windowHeight="16300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5770" yWindow="1260" windowWidth="18900" windowHeight="11770" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Sensitività" sheetId="6" r:id="rId6"/>
     <sheet name="Capacitors" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029" calcCompleted="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="64">
   <si>
     <t>Node</t>
   </si>
@@ -255,6 +255,9 @@
   <si>
     <t>valore iniziale</t>
   </si>
+  <si>
+    <t>angle [rad]</t>
+  </si>
 </sst>
 </file>
 
@@ -327,7 +330,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -337,6 +340,7 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -4378,8 +4382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8A76BB5-5AB4-404D-AE6A-7AC1635BC45D}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5572,20 +5576,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2044FFAD-586E-4B45-A6F7-7B8C372B2BDA}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" customWidth="1"/>
+    <col min="4" max="4" width="9.7265625" customWidth="1"/>
     <col min="6" max="6" width="6.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5595,8 +5600,11 @@
       <c r="C1" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5606,8 +5614,13 @@
       <c r="C2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2">
+        <f>C2*PI()/180</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5617,8 +5630,13 @@
       <c r="C3">
         <v>-4.9564700000000004</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3">
+        <f t="shared" ref="D3:D15" si="0">C3*PI()/180</f>
+        <v>-8.6506720776323348E-2</v>
+      </c>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5628,8 +5646,13 @@
       <c r="C4">
         <v>-12.63274</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>-0.22048290654838848</v>
+      </c>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5639,8 +5662,13 @@
       <c r="C5">
         <v>-10.36585</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>-0.18091821226785421</v>
+      </c>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5650,8 +5678,13 @@
       <c r="C6">
         <v>-8.9466300000000007</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>-0.15614815045770031</v>
+      </c>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5661,8 +5694,13 @@
       <c r="C7">
         <v>-14.87918</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>-0.25969068099688991</v>
+      </c>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -5672,8 +5710,13 @@
       <c r="C8">
         <v>-13.45011</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>-0.23474870425541453</v>
+      </c>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -5683,8 +5726,13 @@
       <c r="C9">
         <v>-13.450049999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>-0.2347476570578633</v>
+      </c>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5694,8 +5742,13 @@
       <c r="C10">
         <v>-15.06968</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>-0.26301553322193905</v>
+      </c>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -5705,8 +5758,13 @@
       <c r="C11">
         <v>-15.31793</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>-0.267348313090015</v>
+      </c>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -5716,8 +5774,13 @@
       <c r="C12">
         <v>-15.213240000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>-0.26552112789610216</v>
+      </c>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -5727,8 +5790,13 @@
       <c r="C13">
         <v>-15.719469999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>-0.27435650816847301</v>
+      </c>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -5738,8 +5806,13 @@
       <c r="C14">
         <v>-15.738060000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>-0.2746809648764188</v>
+      </c>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -5749,6 +5822,11 @@
       <c r="C15">
         <v>-16.39378</v>
       </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>-0.28612543784759598</v>
+      </c>
+      <c r="E15" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>